<commit_message>
update c51e dbc to 0.47 version
</commit_message>
<xml_diff>
--- a/GPIO/RH850D1M1H_176Pin_IO_Config.xlsx
+++ b/GPIO/RH850D1M1H_176Pin_IO_Config.xlsx
@@ -652,9 +652,6 @@
     <t>QSPI_SCK</t>
   </si>
   <si>
-    <t>QSPI_CS</t>
-  </si>
-  <si>
     <t>QSPI_IO0</t>
   </si>
   <si>
@@ -1064,6 +1061,10 @@
   </si>
   <si>
     <t>DIO_08</t>
+  </si>
+  <si>
+    <t>QSPI_CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2826,10 +2827,10 @@
   <dimension ref="A1:AH187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="11" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="H93" sqref="H93"/>
+      <selection pane="bottomRight" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3256,28 +3257,28 @@
         <v>51</v>
       </c>
       <c r="F10" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="G10" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="H10" s="53" t="s">
         <v>272</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="I10" s="53" t="s">
         <v>273</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="J10" s="53" t="s">
         <v>274</v>
       </c>
-      <c r="J10" s="53" t="s">
+      <c r="K10" s="53" t="s">
         <v>275</v>
       </c>
-      <c r="K10" s="53" t="s">
+      <c r="L10" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="L10" s="53" t="s">
+      <c r="M10" s="53" t="s">
         <v>277</v>
-      </c>
-      <c r="M10" s="53" t="s">
-        <v>278</v>
       </c>
       <c r="N10" s="53" t="s">
         <v>96</v>
@@ -3293,28 +3294,28 @@
         <v>51</v>
       </c>
       <c r="S10" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="T10" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="T10" s="53" t="s">
+      <c r="U10" s="53" t="s">
         <v>272</v>
       </c>
-      <c r="U10" s="53" t="s">
+      <c r="V10" s="53" t="s">
         <v>273</v>
       </c>
-      <c r="V10" s="53" t="s">
+      <c r="W10" s="53" t="s">
         <v>274</v>
       </c>
-      <c r="W10" s="53" t="s">
+      <c r="X10" s="53" t="s">
         <v>275</v>
       </c>
-      <c r="X10" s="53" t="s">
+      <c r="Y10" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="Y10" s="53" t="s">
+      <c r="Z10" s="53" t="s">
         <v>277</v>
-      </c>
-      <c r="Z10" s="53" t="s">
-        <v>278</v>
       </c>
       <c r="AA10" s="53" t="s">
         <v>96</v>
@@ -3446,7 +3447,7 @@
       </c>
       <c r="AC12" s="43"/>
       <c r="AD12" s="61" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AE12" s="64">
         <v>8</v>
@@ -3547,7 +3548,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14" s="26">
         <v>0</v>
@@ -3634,7 +3635,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D15" s="26">
         <v>0</v>
@@ -3895,7 +3896,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="26">
         <v>0</v>
@@ -3982,7 +3983,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="26">
         <v>0</v>
@@ -4069,7 +4070,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D20" s="26">
         <v>0</v>
@@ -4156,7 +4157,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D21" s="26">
         <v>0</v>
@@ -4379,7 +4380,7 @@
         <v>56</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D26" s="26">
         <v>0</v>
@@ -4456,7 +4457,7 @@
       </c>
       <c r="AC26" s="43"/>
       <c r="AD26" s="61" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AE26" s="64">
         <v>8</v>
@@ -4470,7 +4471,7 @@
         <v>57</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" s="26">
         <v>0</v>
@@ -4547,7 +4548,7 @@
       </c>
       <c r="AC27" s="43"/>
       <c r="AD27" s="62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AE27" s="64">
         <v>8</v>
@@ -4561,7 +4562,7 @@
         <v>58</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D28" s="26">
         <v>0</v>
@@ -4638,7 +4639,7 @@
       </c>
       <c r="AC28" s="43"/>
       <c r="AD28" s="62" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AE28" s="65">
         <v>8</v>
@@ -4652,7 +4653,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D29" s="26">
         <v>0</v>
@@ -4739,7 +4740,7 @@
         <v>60</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D30" s="26">
         <v>0</v>
@@ -4826,7 +4827,7 @@
         <v>61</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D31" s="26">
         <v>0</v>
@@ -5223,7 +5224,7 @@
         <v>64</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D38" s="26">
         <v>0</v>
@@ -5658,7 +5659,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D43" s="26">
         <v>0</v>
@@ -5832,7 +5833,7 @@
         <v>71</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D45" s="26">
         <v>0</v>
@@ -6838,7 +6839,7 @@
         <v>24</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D59" s="57">
         <v>0</v>
@@ -6925,7 +6926,7 @@
         <v>34</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D60" s="57">
         <v>0</v>
@@ -7002,7 +7003,7 @@
       </c>
       <c r="AC60" s="43"/>
       <c r="AD60" s="62" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AE60" s="64">
         <v>8</v>
@@ -7016,7 +7017,7 @@
         <v>25</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D61" s="57">
         <v>0</v>
@@ -7093,7 +7094,7 @@
       </c>
       <c r="AC61" s="43"/>
       <c r="AD61" s="62" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AE61" s="64">
         <v>8</v>
@@ -7320,7 +7321,7 @@
       </c>
       <c r="AC66" s="43"/>
       <c r="AD66" s="62" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AE66" s="64">
         <v>8</v>
@@ -7411,7 +7412,7 @@
       </c>
       <c r="AC67" s="43"/>
       <c r="AD67" s="62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE67" s="64">
         <v>8</v>
@@ -7735,7 +7736,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D74" s="57">
         <v>1</v>
@@ -7744,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" s="57">
         <v>0</v>
@@ -7822,7 +7823,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D75" s="57">
         <v>1</v>
@@ -7831,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="57">
         <v>0</v>
@@ -7909,7 +7910,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D76" s="57">
         <v>1</v>
@@ -7918,7 +7919,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="57">
         <v>0</v>
@@ -7996,7 +7997,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D77" s="57">
         <v>1</v>
@@ -8005,7 +8006,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" s="57">
         <v>0</v>
@@ -8083,7 +8084,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D78" s="57">
         <v>1</v>
@@ -8092,7 +8093,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="57">
         <v>0</v>
@@ -8170,7 +8171,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D79" s="57">
         <v>1</v>
@@ -8179,7 +8180,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="57">
         <v>0</v>
@@ -8257,7 +8258,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D80" s="57">
         <v>1</v>
@@ -8266,7 +8267,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" s="57">
         <v>0</v>
@@ -8344,7 +8345,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D81" s="57">
         <v>1</v>
@@ -8353,7 +8354,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="57">
         <v>0</v>
@@ -8431,7 +8432,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D82" s="57">
         <v>1</v>
@@ -8440,7 +8441,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="57">
         <v>0</v>
@@ -8518,7 +8519,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D83" s="57">
         <v>1</v>
@@ -8527,7 +8528,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="57">
         <v>0</v>
@@ -8605,7 +8606,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D84" s="57">
         <v>1</v>
@@ -8614,7 +8615,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="57">
         <v>0</v>
@@ -8692,7 +8693,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D85" s="57">
         <v>1</v>
@@ -8701,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="57">
         <v>0</v>
@@ -8915,7 +8916,7 @@
         <v>85</v>
       </c>
       <c r="C90" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D90" s="57">
         <v>0</v>
@@ -8992,7 +8993,7 @@
       </c>
       <c r="AC90" s="49"/>
       <c r="AD90" s="62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE90" s="64">
         <v>8</v>
@@ -9006,7 +9007,7 @@
         <v>82</v>
       </c>
       <c r="C91" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D91" s="57">
         <v>0</v>
@@ -9528,7 +9529,7 @@
         <v>91</v>
       </c>
       <c r="C97" s="50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D97" s="57">
         <v>0</v>
@@ -9702,7 +9703,7 @@
         <v>93</v>
       </c>
       <c r="C99" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D99" s="57">
         <v>0</v>
@@ -9789,7 +9790,7 @@
         <v>94</v>
       </c>
       <c r="C100" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D100" s="57">
         <v>0</v>
@@ -9876,7 +9877,7 @@
         <v>95</v>
       </c>
       <c r="C101" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D101" s="57">
         <v>0</v>
@@ -10042,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" s="57">
         <v>0</v>
@@ -10120,7 +10121,7 @@
         <v>99</v>
       </c>
       <c r="C107" s="50" t="s">
-        <v>188</v>
+        <v>305</v>
       </c>
       <c r="D107" s="57">
         <v>1</v>
@@ -10129,7 +10130,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107" s="57">
         <v>0</v>
@@ -10207,7 +10208,7 @@
         <v>100</v>
       </c>
       <c r="C108" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D108" s="57">
         <v>1</v>
@@ -10294,7 +10295,7 @@
         <v>101</v>
       </c>
       <c r="C109" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D109" s="57">
         <v>1</v>
@@ -10381,7 +10382,7 @@
         <v>102</v>
       </c>
       <c r="C110" s="50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D110" s="57">
         <v>1</v>
@@ -10468,7 +10469,7 @@
         <v>103</v>
       </c>
       <c r="C111" s="50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D111" s="57">
         <v>1</v>
@@ -10555,7 +10556,7 @@
         <v>104</v>
       </c>
       <c r="C112" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D112" s="57">
         <v>0</v>
@@ -10642,7 +10643,7 @@
         <v>105</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D113" s="57">
         <v>0</v>
@@ -10729,7 +10730,7 @@
         <v>106</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D114" s="57">
         <v>0</v>
@@ -10816,7 +10817,7 @@
         <v>107</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D115" s="57">
         <v>0</v>
@@ -10971,7 +10972,7 @@
         <v>108</v>
       </c>
       <c r="C120" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D120" s="57">
         <v>1</v>
@@ -11058,7 +11059,7 @@
         <v>109</v>
       </c>
       <c r="C121" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D121" s="57">
         <v>1</v>
@@ -11145,7 +11146,7 @@
         <v>110</v>
       </c>
       <c r="C122" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D122" s="57">
         <v>1</v>
@@ -11232,7 +11233,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D123" s="57">
         <v>1</v>
@@ -11319,7 +11320,7 @@
         <v>112</v>
       </c>
       <c r="C124" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D124" s="57">
         <v>1</v>
@@ -11406,7 +11407,7 @@
         <v>113</v>
       </c>
       <c r="C125" s="50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D125" s="57">
         <v>1</v>
@@ -11493,7 +11494,7 @@
         <v>114</v>
       </c>
       <c r="C126" s="50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D126" s="57">
         <v>1</v>
@@ -11580,7 +11581,7 @@
         <v>115</v>
       </c>
       <c r="C127" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D127" s="57">
         <v>1</v>
@@ -11667,7 +11668,7 @@
         <v>116</v>
       </c>
       <c r="C128" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D128" s="57">
         <v>1</v>
@@ -11754,7 +11755,7 @@
         <v>117</v>
       </c>
       <c r="C129" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D129" s="57">
         <v>0</v>
@@ -11841,7 +11842,7 @@
         <v>119</v>
       </c>
       <c r="C130" s="50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D130" s="57">
         <v>0</v>
@@ -11928,7 +11929,7 @@
         <v>120</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D131" s="57">
         <v>0</v>
@@ -12015,7 +12016,7 @@
         <v>121</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D132" s="57">
         <v>0</v>
@@ -12102,7 +12103,7 @@
         <v>122</v>
       </c>
       <c r="C133" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D133" s="57">
         <v>0</v>
@@ -12189,7 +12190,7 @@
         <v>123</v>
       </c>
       <c r="C134" s="50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D134" s="57">
         <v>0</v>
@@ -12276,7 +12277,7 @@
         <v>124</v>
       </c>
       <c r="C135" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D135" s="57">
         <v>0</v>
@@ -12431,7 +12432,7 @@
         <v>125</v>
       </c>
       <c r="C140" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D140" s="57">
         <v>0</v>
@@ -12518,7 +12519,7 @@
         <v>118</v>
       </c>
       <c r="C141" s="50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D141" s="57">
         <v>0</v>
@@ -12673,7 +12674,7 @@
         <v>126</v>
       </c>
       <c r="C146" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D146" s="57">
         <v>1</v>
@@ -12760,7 +12761,7 @@
         <v>127</v>
       </c>
       <c r="C147" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D147" s="57">
         <v>1</v>
@@ -12847,7 +12848,7 @@
         <v>128</v>
       </c>
       <c r="C148" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D148" s="57">
         <v>1</v>
@@ -12934,7 +12935,7 @@
         <v>129</v>
       </c>
       <c r="C149" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D149" s="57">
         <v>1</v>
@@ -13021,7 +13022,7 @@
         <v>130</v>
       </c>
       <c r="C150" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D150" s="57">
         <v>1</v>
@@ -13108,7 +13109,7 @@
         <v>131</v>
       </c>
       <c r="C151" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D151" s="57">
         <v>1</v>
@@ -13195,7 +13196,7 @@
         <v>132</v>
       </c>
       <c r="C152" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D152" s="57">
         <v>1</v>
@@ -13282,7 +13283,7 @@
         <v>133</v>
       </c>
       <c r="C153" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D153" s="57">
         <v>1</v>
@@ -13369,7 +13370,7 @@
         <v>134</v>
       </c>
       <c r="C154" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D154" s="57">
         <v>1</v>
@@ -13456,7 +13457,7 @@
         <v>135</v>
       </c>
       <c r="C155" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D155" s="57">
         <v>1</v>
@@ -13543,7 +13544,7 @@
         <v>137</v>
       </c>
       <c r="C156" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D156" s="57">
         <v>1</v>
@@ -13630,7 +13631,7 @@
         <v>138</v>
       </c>
       <c r="C157" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D157" s="57">
         <v>1</v>
@@ -13787,7 +13788,7 @@
         <v>139</v>
       </c>
       <c r="C162" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D162" s="57">
         <v>1</v>
@@ -13874,7 +13875,7 @@
         <v>136</v>
       </c>
       <c r="C163" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D163" s="57">
         <v>1</v>
@@ -13961,7 +13962,7 @@
         <v>140</v>
       </c>
       <c r="C164" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D164" s="57">
         <v>1</v>
@@ -14048,7 +14049,7 @@
         <v>141</v>
       </c>
       <c r="C165" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D165" s="57">
         <v>1</v>
@@ -14135,7 +14136,7 @@
         <v>142</v>
       </c>
       <c r="C166" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D166" s="57">
         <v>1</v>
@@ -14222,7 +14223,7 @@
         <v>143</v>
       </c>
       <c r="C167" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D167" s="57">
         <v>1</v>
@@ -14309,7 +14310,7 @@
         <v>144</v>
       </c>
       <c r="C168" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D168" s="57">
         <v>1</v>
@@ -14396,7 +14397,7 @@
         <v>145</v>
       </c>
       <c r="C169" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D169" s="57">
         <v>1</v>
@@ -14483,7 +14484,7 @@
         <v>146</v>
       </c>
       <c r="C170" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D170" s="57">
         <v>1</v>
@@ -14570,7 +14571,7 @@
         <v>147</v>
       </c>
       <c r="C171" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D171" s="57">
         <v>1</v>
@@ -14657,7 +14658,7 @@
         <v>148</v>
       </c>
       <c r="C172" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D172" s="57">
         <v>1</v>
@@ -14744,7 +14745,7 @@
         <v>149</v>
       </c>
       <c r="C173" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D173" s="57">
         <v>1</v>
@@ -14831,7 +14832,7 @@
         <v>150</v>
       </c>
       <c r="C174" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D174" s="57">
         <v>1</v>
@@ -14918,7 +14919,7 @@
         <v>151</v>
       </c>
       <c r="C175" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D175" s="57">
         <v>1</v>
@@ -15072,10 +15073,10 @@
         <v>5</v>
       </c>
       <c r="B180" s="47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D180" s="26">
         <v>0</v>
@@ -15159,10 +15160,10 @@
         <v>4</v>
       </c>
       <c r="B181" s="47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D181" s="26">
         <v>0</v>
@@ -15246,10 +15247,10 @@
         <v>3</v>
       </c>
       <c r="B182" s="47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D182" s="26">
         <v>0</v>
@@ -15333,10 +15334,10 @@
         <v>2</v>
       </c>
       <c r="B183" s="47" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D183" s="26">
         <v>0</v>
@@ -15420,10 +15421,10 @@
         <v>1</v>
       </c>
       <c r="B184" s="47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D184" s="26">
         <v>0</v>
@@ -15507,10 +15508,10 @@
         <v>176</v>
       </c>
       <c r="B185" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D185" s="26">
         <v>0</v>

</xml_diff>